<commit_message>
Initial commit for 'dataflow-with-document-content' (from Subversion)
</commit_message>
<xml_diff>
--- a/Docs/ATLASDocs.xlsx
+++ b/Docs/ATLASDocs.xlsx
@@ -1,26 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maria/MegaPanDA/DKC/SVNRepository/trunk/Docs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27520" yWindow="6480" windowWidth="28800" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="27525" yWindow="6480" windowWidth="28800" windowHeight="16440" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
     <sheet name="Individuals" sheetId="2" r:id="rId2"/>
     <sheet name="DataSamplesFromTables" sheetId="10" r:id="rId3"/>
+    <sheet name="DatasetCategories" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="485">
   <si>
     <t>Class</t>
   </si>
@@ -640,9 +633,6 @@
     <t>Cross section</t>
   </si>
   <si>
-    <t>Linumosity</t>
-  </si>
-  <si>
     <t>Process</t>
   </si>
   <si>
@@ -1418,13 +1408,82 @@
   </si>
   <si>
     <t>hasGroupCategory</t>
+  </si>
+  <si>
+    <t>Luminosity</t>
+  </si>
+  <si>
+    <t>Unused for now</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>db</t>
+  </si>
+  <si>
+    <t>Database Release</t>
+  </si>
+  <si>
+    <t>calib</t>
+  </si>
+  <si>
+    <t>Calibration</t>
+  </si>
+  <si>
+    <t>cont</t>
+  </si>
+  <si>
+    <t>Physics Container</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>Real Data</t>
+  </si>
+  <si>
+    <t>mc</t>
+  </si>
+  <si>
+    <t>Monte Carlo</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Category full name</t>
+  </si>
+  <si>
+    <t>PDF Analyzer name</t>
+  </si>
+  <si>
+    <t>montecarlo</t>
+  </si>
+  <si>
+    <t>realdata</t>
+  </si>
+  <si>
+    <t>physcont</t>
+  </si>
+  <si>
+    <t>Abbreviation for export</t>
+  </si>
+  <si>
+    <t>calibration</t>
+  </si>
+  <si>
+    <t>database</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1496,6 +1555,15 @@
       <sz val="10.5"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1652,7 +1720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1715,15 +1783,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1734,6 +1793,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2003,7 +2072,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2013,20 +2082,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="5" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" style="6" customWidth="1"/>
-    <col min="5" max="5" width="69.1640625" customWidth="1"/>
+    <col min="5" max="5" width="69.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2040,10 +2109,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -2057,10 +2126,10 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="10" t="s">
         <v>6</v>
@@ -2070,7 +2139,7 @@
       </c>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="10" t="s">
         <v>7</v>
@@ -2082,10 +2151,10 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="10" t="s">
         <v>8</v>
@@ -2097,10 +2166,10 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="10" t="s">
         <v>13</v>
@@ -2112,10 +2181,10 @@
         <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="10" t="s">
         <v>14</v>
@@ -2127,10 +2196,10 @@
         <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="10" t="s">
         <v>15</v>
@@ -2142,10 +2211,10 @@
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="10" t="s">
         <v>16</v>
@@ -2157,10 +2226,10 @@
         <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="10" t="s">
         <v>18</v>
@@ -2172,10 +2241,10 @@
         <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="10" t="s">
         <v>19</v>
@@ -2187,10 +2256,10 @@
         <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="10" t="s">
         <v>20</v>
@@ -2202,10 +2271,10 @@
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="10" t="s">
         <v>21</v>
@@ -2217,10 +2286,10 @@
         <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="10" t="s">
         <v>22</v>
@@ -2232,10 +2301,10 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="10" t="s">
         <v>23</v>
@@ -2247,10 +2316,10 @@
         <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="10" t="s">
         <v>24</v>
@@ -2262,7 +2331,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="10" t="s">
         <v>25</v>
@@ -2274,10 +2343,10 @@
         <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>120</v>
       </c>
@@ -2291,10 +2360,10 @@
         <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="13" t="s">
         <v>121</v>
@@ -2304,7 +2373,7 @@
       </c>
       <c r="D19" s="14"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="13" t="s">
         <v>26</v>
@@ -2316,10 +2385,10 @@
         <v>43</v>
       </c>
       <c r="E20" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="13" t="s">
         <v>27</v>
@@ -2331,10 +2400,10 @@
         <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="13" t="s">
         <v>28</v>
@@ -2346,10 +2415,10 @@
         <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="13" t="s">
         <v>29</v>
@@ -2361,10 +2430,10 @@
         <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>47</v>
       </c>
@@ -2378,10 +2447,10 @@
         <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="16" t="s">
         <v>49</v>
@@ -2393,10 +2462,10 @@
         <v>96</v>
       </c>
       <c r="E25" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="16" t="s">
         <v>50</v>
@@ -2408,10 +2477,10 @@
         <v>95</v>
       </c>
       <c r="E26" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="16" t="s">
         <v>103</v>
@@ -2423,10 +2492,10 @@
         <v>104</v>
       </c>
       <c r="E27" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>51</v>
       </c>
@@ -2443,7 +2512,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="19" t="s">
         <v>52</v>
@@ -2455,10 +2524,10 @@
         <v>99</v>
       </c>
       <c r="E29" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="19" t="s">
         <v>53</v>
@@ -2470,13 +2539,13 @@
         <v>58</v>
       </c>
       <c r="E30" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>12</v>
@@ -2485,10 +2554,10 @@
         <v>59</v>
       </c>
       <c r="E31" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="19" t="s">
         <v>54</v>
@@ -2500,10 +2569,10 @@
         <v>60</v>
       </c>
       <c r="E32" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="19" t="s">
         <v>55</v>
@@ -2515,10 +2584,10 @@
         <v>61</v>
       </c>
       <c r="E33" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="19" t="s">
         <v>56</v>
@@ -2530,10 +2599,10 @@
         <v>62</v>
       </c>
       <c r="E34" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="19" t="s">
         <v>57</v>
@@ -2545,10 +2614,10 @@
         <v>63</v>
       </c>
       <c r="E35" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="19" t="s">
         <v>64</v>
@@ -2560,10 +2629,10 @@
         <v>100</v>
       </c>
       <c r="E36" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="19" t="s">
         <v>65</v>
@@ -2575,10 +2644,10 @@
         <v>73</v>
       </c>
       <c r="E37" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="B38" s="19" t="s">
         <v>66</v>
@@ -2590,10 +2659,10 @@
         <v>74</v>
       </c>
       <c r="E38" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="19" t="s">
         <v>67</v>
@@ -2608,7 +2677,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="19" t="s">
         <v>68</v>
@@ -2620,10 +2689,10 @@
         <v>76</v>
       </c>
       <c r="E40" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
       <c r="B41" s="19" t="s">
         <v>69</v>
@@ -2635,10 +2704,10 @@
         <v>101</v>
       </c>
       <c r="E41" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="19" t="s">
         <v>70</v>
@@ -2650,10 +2719,10 @@
         <v>77</v>
       </c>
       <c r="E42" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="19" t="s">
         <v>71</v>
@@ -2665,10 +2734,10 @@
         <v>78</v>
       </c>
       <c r="E43" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="19" t="s">
         <v>72</v>
@@ -2680,10 +2749,10 @@
         <v>79</v>
       </c>
       <c r="E44" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="19" t="s">
         <v>117</v>
@@ -2693,7 +2762,7 @@
       </c>
       <c r="D45" s="21"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="19" t="s">
         <v>114</v>
@@ -2703,7 +2772,7 @@
       </c>
       <c r="D46" s="21"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="19" t="s">
         <v>115</v>
@@ -2713,7 +2782,7 @@
       </c>
       <c r="D47" s="21"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="19" t="s">
         <v>116</v>
@@ -2721,7 +2790,7 @@
       <c r="C48" s="18"/>
       <c r="D48" s="21"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>80</v>
       </c>
@@ -2735,10 +2804,10 @@
         <v>102</v>
       </c>
       <c r="E49" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
       <c r="B50" s="23" t="s">
         <v>82</v>
@@ -2750,10 +2819,10 @@
         <v>83</v>
       </c>
       <c r="E50" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="26" t="s">
         <v>84</v>
       </c>
@@ -2767,10 +2836,10 @@
         <v>90</v>
       </c>
       <c r="E51" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="26"/>
       <c r="B52" s="27" t="s">
         <v>86</v>
@@ -2782,10 +2851,10 @@
         <v>91</v>
       </c>
       <c r="E52" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="26"/>
       <c r="B53" s="27" t="s">
         <v>87</v>
@@ -2797,10 +2866,10 @@
         <v>92</v>
       </c>
       <c r="E53" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="26"/>
       <c r="B54" s="27" t="s">
         <v>88</v>
@@ -2812,10 +2881,10 @@
         <v>93</v>
       </c>
       <c r="E54" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="26"/>
       <c r="B55" s="27" t="s">
         <v>89</v>
@@ -2827,10 +2896,10 @@
         <v>94</v>
       </c>
       <c r="E55" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
         <v>105</v>
       </c>
@@ -2838,7 +2907,7 @@
       <c r="C56" s="29"/>
       <c r="D56" s="30"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="29" t="s">
         <v>106</v>
       </c>
@@ -2850,7 +2919,7 @@
       </c>
       <c r="D57" s="30"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="29"/>
       <c r="B58" s="31" t="s">
         <v>119</v>
@@ -2860,7 +2929,7 @@
       </c>
       <c r="D58" s="30"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="29"/>
       <c r="B59" s="31" t="s">
         <v>57</v>
@@ -2870,7 +2939,7 @@
       </c>
       <c r="D59" s="30"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="29"/>
       <c r="B60" s="29" t="s">
         <v>56</v>
@@ -2880,7 +2949,7 @@
       </c>
       <c r="D60" s="30"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="29"/>
       <c r="B61" s="29" t="s">
         <v>114</v>
@@ -2890,7 +2959,7 @@
       </c>
       <c r="D61" s="30"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="29"/>
       <c r="B62" s="29" t="s">
         <v>50</v>
@@ -2900,945 +2969,945 @@
       </c>
       <c r="D62" s="30"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="29"/>
       <c r="B63" s="29" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C63" s="29" t="s">
         <v>12</v>
       </c>
       <c r="D63" s="30"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="29"/>
       <c r="B64" s="29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C64" s="29" t="s">
         <v>12</v>
       </c>
       <c r="D64" s="30"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="4"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="4"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="4"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="4"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="4"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="4"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="4"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="4"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="4"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="4"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="4"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="4"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
       <c r="D80" s="4"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
       <c r="D81" s="4"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="4"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
       <c r="D83" s="4"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="4"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="4"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="4"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="4"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="4"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="4"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="4"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="4"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="4"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="4"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="4"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="4"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
       <c r="D99" s="4"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="4"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="4"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="4"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="4"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="4"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="4"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="4"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="4"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="4"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="4"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="4"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="4"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="4"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="4"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="4"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="4"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="4"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="4"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="4"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="4"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="4"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="4"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="4"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="4"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="4"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="4"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="4"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="4"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="4"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="4"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="4"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="4"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
       <c r="D132" s="4"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
       <c r="D133" s="4"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
       <c r="D134" s="4"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
       <c r="D135" s="4"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
       <c r="D136" s="4"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
       <c r="D137" s="4"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
       <c r="D138" s="4"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
       <c r="D139" s="4"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
       <c r="D140" s="4"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
       <c r="D141" s="4"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
       <c r="D142" s="4"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
       <c r="D143" s="4"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
       <c r="D145" s="4"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
       <c r="D146" s="4"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
       <c r="D147" s="4"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
       <c r="D148" s="4"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
       <c r="D149" s="4"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
       <c r="D150" s="4"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
       <c r="D151" s="4"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
       <c r="D152" s="4"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
       <c r="D153" s="4"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
       <c r="D154" s="4"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
       <c r="D155" s="4"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
       <c r="D156" s="4"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
       <c r="D157" s="4"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
       <c r="D158" s="4"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
       <c r="D159" s="4"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
       <c r="D160" s="4"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
       <c r="D161" s="4"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
       <c r="D162" s="4"/>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
       <c r="D163" s="4"/>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
       <c r="D164" s="4"/>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
       <c r="D165" s="4"/>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
       <c r="D166" s="4"/>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
       <c r="D167" s="4"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
       <c r="D168" s="4"/>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
       <c r="D169" s="4"/>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
       <c r="D170" s="4"/>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
       <c r="D171" s="4"/>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
       <c r="D172" s="4"/>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
       <c r="D173" s="4"/>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
       <c r="D174" s="4"/>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
       <c r="D175" s="4"/>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>
       <c r="D176" s="4"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
       <c r="B177" s="3"/>
       <c r="C177" s="3"/>
       <c r="D177" s="4"/>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
       <c r="B178" s="3"/>
       <c r="C178" s="3"/>
       <c r="D178" s="4"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
       <c r="C179" s="3"/>
       <c r="D179" s="4"/>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
       <c r="C180" s="3"/>
       <c r="D180" s="4"/>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
       <c r="B181" s="3"/>
       <c r="C181" s="3"/>
       <c r="D181" s="4"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
       <c r="D182" s="4"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
       <c r="D183" s="4"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
       <c r="D184" s="4"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
       <c r="D185" s="4"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
       <c r="D186" s="4"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
       <c r="D187" s="4"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
       <c r="D188" s="4"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
       <c r="D189" s="4"/>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
       <c r="D190" s="4"/>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
       <c r="D191" s="4"/>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>
       <c r="D192" s="4"/>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="3"/>
       <c r="B193" s="3"/>
       <c r="C193" s="3"/>
       <c r="D193" s="4"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="3"/>
       <c r="B194" s="3"/>
       <c r="C194" s="3"/>
       <c r="D194" s="4"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="3"/>
       <c r="B195" s="3"/>
       <c r="C195" s="3"/>
       <c r="D195" s="4"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="3"/>
       <c r="B196" s="3"/>
       <c r="C196" s="3"/>
       <c r="D196" s="4"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="3"/>
       <c r="B197" s="3"/>
       <c r="C197" s="3"/>
       <c r="D197" s="4"/>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
       <c r="B198" s="3"/>
       <c r="C198" s="3"/>
       <c r="D198" s="4"/>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="3"/>
       <c r="B199" s="3"/>
       <c r="C199" s="3"/>
       <c r="D199" s="4"/>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="3"/>
       <c r="B200" s="3"/>
       <c r="C200" s="3"/>
       <c r="D200" s="4"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="3"/>
       <c r="B201" s="3"/>
       <c r="C201" s="3"/>
       <c r="D201" s="4"/>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="3"/>
       <c r="B202" s="3"/>
       <c r="C202" s="3"/>
       <c r="D202" s="4"/>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="3"/>
       <c r="B203" s="3"/>
       <c r="C203" s="3"/>
       <c r="D203" s="4"/>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="3"/>
       <c r="B204" s="3"/>
       <c r="C204" s="3"/>
       <c r="D204" s="4"/>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="3"/>
       <c r="B205" s="3"/>
       <c r="C205" s="3"/>
       <c r="D205" s="4"/>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="3"/>
       <c r="B206" s="3"/>
       <c r="C206" s="3"/>
       <c r="D206" s="4"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="3"/>
       <c r="B207" s="3"/>
       <c r="C207" s="3"/>
       <c r="D207" s="4"/>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="3"/>
       <c r="B208" s="3"/>
       <c r="C208" s="3"/>
       <c r="D208" s="4"/>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="3"/>
       <c r="B209" s="3"/>
       <c r="C209" s="3"/>
       <c r="D209" s="4"/>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="3"/>
       <c r="B210" s="3"/>
       <c r="C210" s="3"/>
       <c r="D210" s="4"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="3"/>
       <c r="B211" s="3"/>
       <c r="C211" s="3"/>
       <c r="D211" s="4"/>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="3"/>
       <c r="B212" s="3"/>
       <c r="C212" s="3"/>
       <c r="D212" s="4"/>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="3"/>
       <c r="B213" s="3"/>
       <c r="C213" s="3"/>
       <c r="D213" s="4"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="3"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
       <c r="D214" s="4"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="3"/>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
       <c r="D215" s="4"/>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="3"/>
       <c r="B216" s="3"/>
       <c r="C216" s="3"/>
       <c r="D216" s="4"/>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="3"/>
       <c r="B217" s="3"/>
       <c r="C217" s="3"/>
       <c r="D217" s="4"/>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="3"/>
       <c r="B218" s="3"/>
       <c r="C218" s="3"/>
@@ -3858,20 +3927,20 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.625" customWidth="1"/>
+    <col min="4" max="4" width="27.625" customWidth="1"/>
+    <col min="5" max="5" width="19.625" customWidth="1"/>
     <col min="8" max="8" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
-        <v>438</v>
+    <row r="1" spans="1:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="39" t="s">
+        <v>437</v>
       </c>
       <c r="B1" s="32" t="s">
         <v>183</v>
@@ -3898,18 +3967,18 @@
         <v>190</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>439</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>443</v>
+        <v>438</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>442</v>
       </c>
       <c r="C2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E2" t="s">
         <v>132</v>
@@ -3927,18 +3996,18 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>440</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>444</v>
+        <v>439</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>443</v>
       </c>
       <c r="C3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E3" t="s">
         <v>133</v>
@@ -3956,18 +4025,18 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>441</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>445</v>
+        <v>440</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>444</v>
       </c>
       <c r="C4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E4" t="s">
         <v>134</v>
@@ -3985,18 +4054,18 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>442</v>
-      </c>
-      <c r="B5" s="40" t="s">
-        <v>446</v>
+        <v>441</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>445</v>
       </c>
       <c r="C5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E5" t="s">
         <v>135</v>
@@ -4011,15 +4080,15 @@
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="41" t="s">
-        <v>447</v>
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="38" t="s">
+        <v>446</v>
       </c>
       <c r="C6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E6" t="s">
         <v>136</v>
@@ -4034,15 +4103,15 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
-        <v>456</v>
+    <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="37" t="s">
+        <v>455</v>
       </c>
       <c r="C7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E7" t="s">
         <v>137</v>
@@ -4057,15 +4126,15 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41" t="s">
+    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="38" t="s">
         <v>131</v>
       </c>
       <c r="C8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E8" t="s">
         <v>138</v>
@@ -4080,12 +4149,12 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E9" t="s">
         <v>139</v>
@@ -4100,12 +4169,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="41" t="s">
-        <v>448</v>
+    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="38" t="s">
+        <v>447</v>
       </c>
       <c r="D10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E10" t="s">
         <v>140</v>
@@ -4117,29 +4186,29 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
-        <v>449</v>
+    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="37" t="s">
+        <v>448</v>
       </c>
       <c r="D11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E11" t="s">
         <v>141</v>
       </c>
       <c r="F11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="s">
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="38" t="s">
         <v>125</v>
       </c>
       <c r="D12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E12" t="s">
         <v>142</v>
@@ -4148,12 +4217,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="40" t="s">
-        <v>450</v>
+    <row r="13" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="37" t="s">
+        <v>449</v>
       </c>
       <c r="D13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E13" t="s">
         <v>143</v>
@@ -4162,12 +4231,12 @@
         <v>174</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="41" t="s">
+    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="38" t="s">
         <v>129</v>
       </c>
       <c r="D14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E14" t="s">
         <v>144</v>
@@ -4176,15 +4245,15 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="40" t="s">
-        <v>451</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>423</v>
+    <row r="15" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="37" t="s">
+        <v>450</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>422</v>
       </c>
       <c r="D15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E15" t="s">
         <v>145</v>
@@ -4193,15 +4262,15 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="41" t="s">
+    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="38" t="s">
         <v>123</v>
       </c>
       <c r="C16" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E16" t="s">
         <v>146</v>
@@ -4210,15 +4279,15 @@
         <v>177</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="40" t="s">
+    <row r="17" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="37" t="s">
         <v>124</v>
       </c>
       <c r="C17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E17" t="s">
         <v>147</v>
@@ -4227,15 +4296,15 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="41" t="s">
-        <v>452</v>
+    <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="38" t="s">
+        <v>451</v>
       </c>
       <c r="C18" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E18" t="s">
         <v>148</v>
@@ -4244,825 +4313,825 @@
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+    <row r="19" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="37" t="s">
         <v>128</v>
       </c>
       <c r="C19" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E19" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="41" t="s">
+    <row r="20" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="38" t="s">
         <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E20" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="40" t="s">
-        <v>457</v>
+    <row r="21" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="37" t="s">
+        <v>456</v>
       </c>
       <c r="C21" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E21" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="41" t="s">
+    <row r="22" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="38" t="s">
         <v>122</v>
       </c>
       <c r="C22" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E22" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="40" t="s">
-        <v>453</v>
+    <row r="23" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="37" t="s">
+        <v>452</v>
       </c>
       <c r="C23" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E23" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="41" t="s">
+    <row r="24" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="38" t="s">
+        <v>453</v>
+      </c>
+      <c r="C24" t="s">
+        <v>431</v>
+      </c>
+      <c r="D24" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="37" t="s">
+        <v>457</v>
+      </c>
+      <c r="C25" t="s">
+        <v>432</v>
+      </c>
+      <c r="D25" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" t="s">
+        <v>433</v>
+      </c>
+      <c r="D26" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" t="s">
+        <v>434</v>
+      </c>
+      <c r="D27" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="38" t="s">
+        <v>458</v>
+      </c>
+      <c r="C28" t="s">
+        <v>435</v>
+      </c>
+      <c r="D28" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="37" t="s">
         <v>454</v>
       </c>
-      <c r="C24" t="s">
-        <v>432</v>
-      </c>
-      <c r="D24" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="40" t="s">
-        <v>458</v>
-      </c>
-      <c r="C25" t="s">
-        <v>433</v>
-      </c>
-      <c r="D25" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="41" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" t="s">
-        <v>434</v>
-      </c>
-      <c r="D26" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" t="s">
-        <v>435</v>
-      </c>
-      <c r="D27" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="41" t="s">
-        <v>459</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>436</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="40" t="s">
-        <v>455</v>
-      </c>
-      <c r="C29" t="s">
-        <v>437</v>
-      </c>
-      <c r="D29" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D30" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D31" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D32" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D33" t="s">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D34" t="s">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" t="s">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D36" t="s">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D37" t="s">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D38" t="s">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D39" t="s">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D40" t="s">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D41" t="s">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D42" t="s">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D43" t="s">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D45" t="s">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D46" t="s">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D47" t="s">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D48" t="s">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D49" t="s">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D50" t="s">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D51" t="s">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D52" t="s">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D53" t="s">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D54" t="s">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D55" t="s">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D56" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D57" t="s">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D58" t="s">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D59" t="s">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D61" t="s">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D62" t="s">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D63" t="s">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D64" t="s">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D65" t="s">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D66" t="s">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D67" t="s">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D68" t="s">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D69" t="s">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D70" t="s">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D71" t="s">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D72" t="s">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D73" t="s">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D74" t="s">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D75" t="s">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D76" t="s">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D77" t="s">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D78" t="s">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D79" t="s">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D80" t="s">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D81" t="s">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D82" t="s">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D83" t="s">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D84" t="s">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D85" t="s">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D86" t="s">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D87" t="s">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D88" t="s">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D89" t="s">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D90" t="s">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D91" t="s">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D92" t="s">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D93" t="s">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D94" t="s">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D95" t="s">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D96" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D96" t="s">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D97" t="s">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D98" t="s">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D99" t="s">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D100" t="s">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D101" t="s">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D102" t="s">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D103" t="s">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D104" t="s">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D105" t="s">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D106" t="s">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D107" t="s">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D108" t="s">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D109" t="s">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D110" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D110" t="s">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D111" t="s">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D112" t="s">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D113" t="s">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D114" t="s">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D115" t="s">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D116" t="s">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D117" t="s">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D118" t="s">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D119" t="s">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D120" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D120" t="s">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D121" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D121" t="s">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D122" t="s">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D123" t="s">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D124" t="s">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D125" t="s">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D126" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D126" t="s">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D127" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D127" t="s">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D128" t="s">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D129" t="s">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D130" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D130" t="s">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D131" t="s">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D132" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D132" t="s">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D133" t="s">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D134" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D134" t="s">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D135" t="s">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D136" t="s">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D137" t="s">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D138" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D138" t="s">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D139" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D139" t="s">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D140" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D140" t="s">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D141" t="s">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D142" t="s">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D143" t="s">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D144" t="s">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D145" t="s">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D146" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D146" t="s">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D147" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D147" t="s">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D148" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D148" t="s">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D149" t="s">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D150" t="s">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D151" t="s">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D152" t="s">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D153" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D153" t="s">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D154" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D154" t="s">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D155" t="s">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D156" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D156" t="s">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D157" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D157" t="s">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D158" t="s">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D159" t="s">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D160" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D160" t="s">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D161" t="s">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D162" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D162" t="s">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D163" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D163" t="s">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D164" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D164" t="s">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D165" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D165" t="s">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D166" t="s">
         <v>419</v>
-      </c>
-    </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D166" t="s">
-        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -5075,57 +5144,57 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="2" max="2" width="23.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="40" t="s">
         <v>199</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="37"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="41"/>
       <c r="B3" s="5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="37"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="41"/>
       <c r="B4" s="5" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="41"/>
       <c r="B5" s="5" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="37"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="41"/>
       <c r="B6" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="38"/>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="42"/>
       <c r="B7" s="5" t="s">
         <v>197</v>
       </c>
@@ -5134,60 +5203,60 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="36" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
         <v>198</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
       <c r="B10" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="41"/>
       <c r="B11" s="5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="41"/>
       <c r="B12" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="37"/>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="41"/>
       <c r="B13" s="5" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="37"/>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
       <c r="B14" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="41"/>
+      <c r="B15" s="5" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="37"/>
-      <c r="B15" s="5" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="41"/>
+      <c r="B16" s="5" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="37"/>
-      <c r="B16" s="5" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="42"/>
+      <c r="B17" s="5" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="38"/>
-      <c r="B17" s="5" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -5197,4 +5266,123 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" customWidth="1"/>
+    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>477</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>482</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B3" t="s">
+        <v>480</v>
+      </c>
+      <c r="C3" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>471</v>
+      </c>
+      <c r="B4" t="s">
+        <v>481</v>
+      </c>
+      <c r="C4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B5" t="s">
+        <v>483</v>
+      </c>
+      <c r="C5" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>467</v>
+      </c>
+      <c r="B6" t="s">
+        <v>484</v>
+      </c>
+      <c r="C6" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>465</v>
+      </c>
+      <c r="B7" t="s">
+        <v>356</v>
+      </c>
+      <c r="C7" t="s">
+        <v>356</v>
+      </c>
+      <c r="D7" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>464</v>
+      </c>
+      <c r="B8" t="s">
+        <v>414</v>
+      </c>
+      <c r="C8" t="s">
+        <v>414</v>
+      </c>
+      <c r="D8" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>